<commit_message>
Data analysis almost completed. Report being written.
</commit_message>
<xml_diff>
--- a/results/TokenCardICODistribution.xlsx
+++ b/results/TokenCardICODistribution.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28080" windowHeight="16820" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="640" yWindow="1180" windowWidth="28080" windowHeight="16820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5815" uniqueCount="1591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5820" uniqueCount="1596">
   <si>
     <t>Account</t>
   </si>
@@ -4805,6 +4805,21 @@
   </si>
   <si>
     <t>Was not picked up by my script</t>
+  </si>
+  <si>
+    <t>SNGLS/ETH</t>
+  </si>
+  <si>
+    <t>Tokens should be</t>
+  </si>
+  <si>
+    <t>Tokens allocated</t>
+  </si>
+  <si>
+    <t>Total tokens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total tokens should have been </t>
   </si>
 </sst>
 </file>
@@ -5032,7 +5047,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5052,6 +5067,10 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="79">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -5134,17 +5153,7 @@
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5441,8 +5450,8 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:M1857"/>
   <sheetViews>
-    <sheetView topLeftCell="A725" workbookViewId="0">
-      <selection sqref="A1:M1840"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1764" sqref="D1764"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5651,7 +5660,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>171</v>
       </c>
@@ -6335,7 +6344,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>1453</v>
       </c>
@@ -6639,7 +6648,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>144</v>
       </c>
@@ -6791,7 +6800,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>147</v>
       </c>
@@ -7326,7 +7335,7 @@
         <v>1566</v>
       </c>
     </row>
-    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>86</v>
       </c>
@@ -7478,7 +7487,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>165</v>
       </c>
@@ -7668,7 +7677,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>1455</v>
       </c>
@@ -8280,7 +8289,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>94</v>
       </c>
@@ -8778,7 +8787,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>1496</v>
       </c>
@@ -8816,7 +8825,7 @@
         <v>1567</v>
       </c>
     </row>
-    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>114</v>
       </c>
@@ -8934,7 +8943,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="92" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>130</v>
       </c>
@@ -9010,7 +9019,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>90</v>
       </c>
@@ -9048,7 +9057,7 @@
         <v>1562</v>
       </c>
     </row>
-    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>173</v>
       </c>
@@ -9124,7 +9133,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>892</v>
       </c>
@@ -9470,7 +9479,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>1494</v>
       </c>
@@ -9812,7 +9821,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>69</v>
       </c>
@@ -10009,7 +10018,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>95</v>
       </c>
@@ -10089,7 +10098,7 @@
         <v>1566</v>
       </c>
     </row>
-    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>116</v>
       </c>
@@ -10431,7 +10440,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>654</v>
       </c>
@@ -12072,7 +12081,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>133</v>
       </c>
@@ -12452,7 +12461,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="184" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>146</v>
       </c>
@@ -13102,7 +13111,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" s="5" t="s">
         <v>745</v>
       </c>
@@ -13182,7 +13191,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" s="5" t="s">
         <v>745</v>
       </c>
@@ -13714,7 +13723,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="217" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A217" s="2" t="s">
         <v>136</v>
       </c>
@@ -13756,7 +13765,7 @@
         <v>12.174662976</v>
       </c>
     </row>
-    <row r="218" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A218" s="2" t="s">
         <v>136</v>
       </c>
@@ -13946,7 +13955,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223" s="5" t="s">
         <v>887</v>
       </c>
@@ -14064,7 +14073,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="226" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>85</v>
       </c>
@@ -14634,7 +14643,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" s="2" t="s">
         <v>1086</v>
       </c>
@@ -16211,7 +16220,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="282" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A282" s="2" t="s">
         <v>155</v>
       </c>
@@ -16291,7 +16300,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="284" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>153</v>
       </c>
@@ -16557,7 +16566,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="291" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>159</v>
       </c>
@@ -16633,7 +16642,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="293" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>118</v>
       </c>
@@ -17169,7 +17178,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="307" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A307" s="2" t="s">
         <v>32</v>
       </c>
@@ -17933,7 +17942,7 @@
         <v>2584.2919999999999</v>
       </c>
     </row>
-    <row r="327" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A327" s="5" t="s">
         <v>604</v>
       </c>
@@ -18123,7 +18132,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="332" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>1502</v>
       </c>
@@ -18237,7 +18246,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="335" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A335" s="2" t="s">
         <v>1053</v>
       </c>
@@ -18431,7 +18440,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="340" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>1466</v>
       </c>
@@ -18735,7 +18744,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="348" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>177</v>
       </c>
@@ -19385,7 +19394,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="365" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>132</v>
       </c>
@@ -20947,7 +20956,7 @@
         <v>364.46</v>
       </c>
     </row>
-    <row r="406" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A406" s="2" t="s">
         <v>436</v>
       </c>
@@ -21213,7 +21222,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="413" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A413" s="2" t="s">
         <v>1061</v>
       </c>
@@ -21749,7 +21758,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="427" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A427" t="s">
         <v>156</v>
       </c>
@@ -21901,7 +21910,7 @@
         <v>1569</v>
       </c>
     </row>
-    <row r="431" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
         <v>76</v>
       </c>
@@ -22281,7 +22290,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="441" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A441" s="2" t="s">
         <v>1533</v>
       </c>
@@ -22516,7 +22525,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="447" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A447" t="s">
         <v>139</v>
       </c>
@@ -22630,7 +22639,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="450" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A450" t="s">
         <v>1521</v>
       </c>
@@ -22744,7 +22753,7 @@
         <v>1566</v>
       </c>
     </row>
-    <row r="453" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A453" s="6" t="s">
         <v>99</v>
       </c>
@@ -22786,7 +22795,7 @@
         <v>57.692010866999993</v>
       </c>
     </row>
-    <row r="454" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A454" s="6" t="s">
         <v>99</v>
       </c>
@@ -22824,7 +22833,7 @@
         <v>1562</v>
       </c>
     </row>
-    <row r="455" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A455" s="6" t="s">
         <v>99</v>
       </c>
@@ -23474,7 +23483,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="472" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A472" t="s">
         <v>1547</v>
       </c>
@@ -23553,7 +23562,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="474" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A474" t="s">
         <v>80</v>
       </c>
@@ -23591,7 +23600,7 @@
         <v>1562</v>
       </c>
     </row>
-    <row r="475" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A475" t="s">
         <v>84</v>
       </c>
@@ -23819,7 +23828,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="481" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A481" s="5" t="s">
         <v>91</v>
       </c>
@@ -24127,7 +24136,7 @@
         <v>1566</v>
       </c>
     </row>
-    <row r="489" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="489" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A489" s="2" t="s">
         <v>1483</v>
       </c>
@@ -24168,7 +24177,7 @@
         <v>1584</v>
       </c>
     </row>
-    <row r="490" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A490" s="2" t="s">
         <v>1483</v>
       </c>
@@ -24704,7 +24713,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="504" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="504" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A504" t="s">
         <v>1516</v>
       </c>
@@ -24932,7 +24941,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="510" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="510" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A510" t="s">
         <v>160</v>
       </c>
@@ -25920,7 +25929,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="536" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="536" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A536" t="s">
         <v>148</v>
       </c>
@@ -25958,7 +25967,7 @@
         <v>1562</v>
       </c>
     </row>
-    <row r="537" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="537" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A537" t="s">
         <v>141</v>
       </c>
@@ -26608,7 +26617,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="554" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="554" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A554" t="s">
         <v>83</v>
       </c>
@@ -26874,7 +26883,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="561" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="561" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A561" t="s">
         <v>1512</v>
       </c>
@@ -26950,7 +26959,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="563" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="563" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A563" t="s">
         <v>107</v>
       </c>
@@ -27102,7 +27111,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="567" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="567" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A567" t="s">
         <v>1448</v>
       </c>
@@ -27368,7 +27377,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="574" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="574" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A574" t="s">
         <v>115</v>
       </c>
@@ -27976,7 +27985,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="590" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="590" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A590" s="2" t="s">
         <v>96</v>
       </c>
@@ -28360,7 +28369,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="600" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="600" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A600" t="s">
         <v>1529</v>
       </c>
@@ -28512,7 +28521,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="604" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="604" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A604" t="s">
         <v>74</v>
       </c>
@@ -28816,7 +28825,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="612" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="612" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A612" s="2" t="s">
         <v>344</v>
       </c>
@@ -29055,7 +29064,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="618" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="618" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A618" s="5" t="s">
         <v>191</v>
       </c>
@@ -29169,7 +29178,7 @@
         <v>1569</v>
       </c>
     </row>
-    <row r="621" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="621" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A621" t="s">
         <v>167</v>
       </c>
@@ -29207,7 +29216,7 @@
         <v>1562</v>
       </c>
     </row>
-    <row r="622" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="622" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A622" t="s">
         <v>110</v>
       </c>
@@ -30385,7 +30394,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="653" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="653" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A653" s="2" t="s">
         <v>128</v>
       </c>
@@ -30503,7 +30512,7 @@
         <v>1569</v>
       </c>
     </row>
-    <row r="656" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="656" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A656" t="s">
         <v>79</v>
       </c>
@@ -31115,7 +31124,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="672" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="672" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A672" t="s">
         <v>1465</v>
       </c>
@@ -31267,7 +31276,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="676" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="676" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A676" s="2" t="s">
         <v>87</v>
       </c>
@@ -31617,7 +31626,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="685" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="685" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A685" t="s">
         <v>81</v>
       </c>
@@ -32263,7 +32272,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="702" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="702" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A702" t="s">
         <v>150</v>
       </c>
@@ -32989,7 +32998,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="721" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="721" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A721" t="s">
         <v>98</v>
       </c>
@@ -33141,7 +33150,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="725" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="725" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A725" s="2" t="s">
         <v>859</v>
       </c>
@@ -33867,7 +33876,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="744" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="744" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A744" t="s">
         <v>1480</v>
       </c>
@@ -34361,7 +34370,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="757" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="757" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A757" t="s">
         <v>1535</v>
       </c>
@@ -34399,7 +34408,7 @@
         <v>1567</v>
       </c>
     </row>
-    <row r="758" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="758" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A758" s="2" t="s">
         <v>125</v>
       </c>
@@ -34821,7 +34830,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="769" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="769" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A769" t="s">
         <v>1534</v>
       </c>
@@ -35809,7 +35818,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="795" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="795" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A795" t="s">
         <v>1468</v>
       </c>
@@ -35847,7 +35856,7 @@
         <v>1567</v>
       </c>
     </row>
-    <row r="796" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="796" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A796" s="2" t="s">
         <v>1161</v>
       </c>
@@ -36155,7 +36164,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="804" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="804" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A804" t="s">
         <v>157</v>
       </c>
@@ -36193,7 +36202,7 @@
         <v>1562</v>
       </c>
     </row>
-    <row r="805" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="805" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A805" t="s">
         <v>152</v>
       </c>
@@ -36573,7 +36582,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="815" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="815" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A815" t="s">
         <v>126</v>
       </c>
@@ -36804,7 +36813,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="821" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="821" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A821" t="s">
         <v>122</v>
       </c>
@@ -37526,7 +37535,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="840" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="840" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A840" t="s">
         <v>1487</v>
       </c>
@@ -37678,7 +37687,7 @@
         <v>1565</v>
       </c>
     </row>
-    <row r="844" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="844" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A844" t="s">
         <v>140</v>
       </c>
@@ -37792,7 +37801,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="847" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="847" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A847" t="s">
         <v>1464</v>
       </c>
@@ -38476,7 +38485,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="865" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="865" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A865" t="s">
         <v>138</v>
       </c>
@@ -39084,7 +39093,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="881" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="881" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A881" t="s">
         <v>1457</v>
       </c>
@@ -39122,7 +39131,7 @@
         <v>1567</v>
       </c>
     </row>
-    <row r="882" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="882" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A882" t="s">
         <v>113</v>
       </c>
@@ -39160,7 +39169,7 @@
         <v>1562</v>
       </c>
     </row>
-    <row r="883" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="883" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A883" s="2" t="s">
         <v>767</v>
       </c>
@@ -40038,7 +40047,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="906" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="906" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A906" t="s">
         <v>129</v>
       </c>
@@ -41178,7 +41187,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="936" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="936" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A936" t="s">
         <v>104</v>
       </c>
@@ -41406,7 +41415,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="942" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="942" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A942" t="s">
         <v>119</v>
       </c>
@@ -43160,7 +43169,7 @@
         <v>1588</v>
       </c>
     </row>
-    <row r="988" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="988" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A988" t="s">
         <v>120</v>
       </c>
@@ -43692,7 +43701,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1002" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1002" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1002" s="2" t="s">
         <v>163</v>
       </c>
@@ -44152,7 +44161,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1014" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1014" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1014" s="2" t="s">
         <v>89</v>
       </c>
@@ -44194,7 +44203,7 @@
         <v>23.150000000000002</v>
       </c>
     </row>
-    <row r="1015" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1015" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1015" s="2" t="s">
         <v>89</v>
       </c>
@@ -44346,7 +44355,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1019" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1019" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1019" t="s">
         <v>67</v>
       </c>
@@ -44878,7 +44887,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1033" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1033" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1033" t="s">
         <v>143</v>
       </c>
@@ -45831,7 +45840,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1058" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1058" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1058" t="s">
         <v>170</v>
       </c>
@@ -46135,7 +46144,7 @@
         <v>1566</v>
       </c>
     </row>
-    <row r="1066" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1066" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1066" t="s">
         <v>70</v>
       </c>
@@ -46591,7 +46600,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1078" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1078" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1078" t="s">
         <v>112</v>
       </c>
@@ -47541,7 +47550,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1103" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1103" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1103" t="s">
         <v>1463</v>
       </c>
@@ -47731,7 +47740,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1108" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1108" t="s">
         <v>108</v>
       </c>
@@ -48233,7 +48242,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1121" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1121" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1121" t="s">
         <v>1548</v>
       </c>
@@ -48958,7 +48967,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1140" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1140" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1140" t="s">
         <v>168</v>
       </c>
@@ -49072,7 +49081,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1143" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1143" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1143" t="s">
         <v>166</v>
       </c>
@@ -49414,7 +49423,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1152" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1152" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1152" s="5" t="s">
         <v>1501</v>
       </c>
@@ -49456,7 +49465,7 @@
         <v>9962.32</v>
       </c>
     </row>
-    <row r="1153" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1153" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1153" s="5" t="s">
         <v>1501</v>
       </c>
@@ -49760,7 +49769,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1161" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1161" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1161" t="s">
         <v>117</v>
       </c>
@@ -50596,7 +50605,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1183" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1183" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1183" t="s">
         <v>1459</v>
       </c>
@@ -50900,7 +50909,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1191" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1191" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1191" t="s">
         <v>111</v>
       </c>
@@ -50976,7 +50985,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1193" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1193" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1193" t="s">
         <v>1522</v>
       </c>
@@ -51546,7 +51555,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1208" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1208" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1208" t="s">
         <v>106</v>
       </c>
@@ -52572,7 +52581,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1235" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1235" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1235" s="2" t="s">
         <v>651</v>
       </c>
@@ -53184,7 +53193,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1251" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1251" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1251" t="s">
         <v>1530</v>
       </c>
@@ -53754,7 +53763,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1266" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1266" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1266" t="s">
         <v>66</v>
       </c>
@@ -53830,7 +53839,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1268" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1268" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1268" t="s">
         <v>82</v>
       </c>
@@ -54210,7 +54219,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1278" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1278" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1278" t="s">
         <v>162</v>
       </c>
@@ -54666,7 +54675,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1290" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1290" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1290" t="s">
         <v>1473</v>
       </c>
@@ -54970,7 +54979,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1298" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1298" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1298" t="s">
         <v>124</v>
       </c>
@@ -55962,7 +55971,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1324" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1324" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1324" s="2" t="s">
         <v>886</v>
       </c>
@@ -56156,7 +56165,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1329" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1329" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1329" s="2" t="s">
         <v>691</v>
       </c>
@@ -56768,7 +56777,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1345" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1345" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1345" t="s">
         <v>92</v>
       </c>
@@ -57262,7 +57271,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1358" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1358" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1358" t="s">
         <v>176</v>
       </c>
@@ -57946,7 +57955,7 @@
         <v>1566</v>
       </c>
     </row>
-    <row r="1376" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1376" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1376" t="s">
         <v>88</v>
       </c>
@@ -58478,7 +58487,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1390" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1390" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1390" t="s">
         <v>164</v>
       </c>
@@ -58672,7 +58681,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1395" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1395" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1395" t="s">
         <v>109</v>
       </c>
@@ -58862,7 +58871,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1400" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1400" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1400" t="s">
         <v>73</v>
       </c>
@@ -58938,7 +58947,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1402" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1402" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1402" t="s">
         <v>103</v>
       </c>
@@ -59204,7 +59213,7 @@
         <v>1569</v>
       </c>
     </row>
-    <row r="1409" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1409" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1409" t="s">
         <v>169</v>
       </c>
@@ -59816,7 +59825,7 @@
         <v>401.87</v>
       </c>
     </row>
-    <row r="1425" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1425" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1425" s="5" t="s">
         <v>234</v>
       </c>
@@ -60196,7 +60205,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1435" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1435" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1435" t="s">
         <v>68</v>
       </c>
@@ -61526,7 +61535,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1470" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1470" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1470" s="5" t="s">
         <v>1176</v>
       </c>
@@ -61723,7 +61732,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1475" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1475" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1475" t="s">
         <v>101</v>
       </c>
@@ -61951,7 +61960,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1481" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1481" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1481" t="s">
         <v>1481</v>
       </c>
@@ -62141,7 +62150,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1486" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1486" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1486" s="2" t="s">
         <v>185</v>
       </c>
@@ -62449,7 +62458,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1494" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1494" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1494" t="s">
         <v>135</v>
       </c>
@@ -62639,7 +62648,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1499" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1499" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1499" t="s">
         <v>158</v>
       </c>
@@ -63323,7 +63332,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1517" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1517" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1517" t="s">
         <v>137</v>
       </c>
@@ -63399,7 +63408,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1519" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1519" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1519" t="s">
         <v>105</v>
       </c>
@@ -63589,7 +63598,7 @@
         <v>1569</v>
       </c>
     </row>
-    <row r="1524" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1524" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1524" t="s">
         <v>131</v>
       </c>
@@ -63703,7 +63712,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1527" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1527" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1527" t="s">
         <v>1476</v>
       </c>
@@ -64577,7 +64586,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1550" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1550" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1550" t="s">
         <v>1482</v>
       </c>
@@ -65155,7 +65164,7 @@
         <v>32.554000000000002</v>
       </c>
     </row>
-    <row r="1565" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1565" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1565" s="5" t="s">
         <v>100</v>
       </c>
@@ -65725,7 +65734,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1580" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1580" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1580" t="s">
         <v>127</v>
       </c>
@@ -65763,7 +65772,7 @@
         <v>1562</v>
       </c>
     </row>
-    <row r="1581" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1581" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1581" t="s">
         <v>149</v>
       </c>
@@ -66151,7 +66160,7 @@
         <v>41.214559999999999</v>
       </c>
     </row>
-    <row r="1591" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1591" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1591" s="2" t="s">
         <v>792</v>
       </c>
@@ -66379,7 +66388,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1597" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1597" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1597" t="s">
         <v>142</v>
       </c>
@@ -66455,7 +66464,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1599" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1599" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1599" t="s">
         <v>175</v>
       </c>
@@ -66531,7 +66540,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1601" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1601" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1601" t="s">
         <v>1471</v>
       </c>
@@ -67101,7 +67110,7 @@
         <v>1566</v>
       </c>
     </row>
-    <row r="1616" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1616" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1616" t="s">
         <v>121</v>
       </c>
@@ -67606,7 +67615,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1629" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1629" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1629" t="s">
         <v>65</v>
       </c>
@@ -68366,7 +68375,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1649" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1649" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1649" s="2" t="s">
         <v>75</v>
       </c>
@@ -69054,7 +69063,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1667" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1667" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1667" t="s">
         <v>161</v>
       </c>
@@ -69552,7 +69561,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1680" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1680" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1680" s="2" t="s">
         <v>1076</v>
       </c>
@@ -69670,7 +69679,7 @@
         <v>1566</v>
       </c>
     </row>
-    <row r="1683" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1683" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1683" t="s">
         <v>1488</v>
       </c>
@@ -69822,7 +69831,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1687" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1687" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1687" t="s">
         <v>97</v>
       </c>
@@ -69860,7 +69869,7 @@
         <v>1562</v>
       </c>
     </row>
-    <row r="1688" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1688" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1688" t="s">
         <v>1513</v>
       </c>
@@ -70620,7 +70629,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1708" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1708" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1708" t="s">
         <v>1490</v>
       </c>
@@ -70810,7 +70819,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1713" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1713" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1713" s="2" t="s">
         <v>1500</v>
       </c>
@@ -70848,7 +70857,7 @@
         <v>1567</v>
       </c>
     </row>
-    <row r="1714" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1714" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1714" s="2" t="s">
         <v>1500</v>
       </c>
@@ -72068,7 +72077,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1746" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1746" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1746" t="s">
         <v>71</v>
       </c>
@@ -72448,7 +72457,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1756" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1756" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1756" t="s">
         <v>77</v>
       </c>
@@ -72752,7 +72761,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1764" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1764" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1764" t="s">
         <v>172</v>
       </c>
@@ -73436,7 +73445,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1782" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1782" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1782" t="s">
         <v>64</v>
       </c>
@@ -73474,7 +73483,7 @@
         <v>1562</v>
       </c>
     </row>
-    <row r="1783" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1783" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1783" t="s">
         <v>93</v>
       </c>
@@ -73702,7 +73711,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1789" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1789" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1789" t="s">
         <v>154</v>
       </c>
@@ -73933,7 +73942,7 @@
         <v>1589</v>
       </c>
     </row>
-    <row r="1795" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1795" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1795" t="s">
         <v>72</v>
       </c>
@@ -73971,7 +73980,7 @@
         <v>1562</v>
       </c>
     </row>
-    <row r="1796" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1796" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1796" t="s">
         <v>78</v>
       </c>
@@ -74047,7 +74056,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1798" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1798" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1798" t="s">
         <v>174</v>
       </c>
@@ -74275,7 +74284,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1804" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1804" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1804" t="s">
         <v>1539</v>
       </c>
@@ -74313,7 +74322,7 @@
         <v>1567</v>
       </c>
     </row>
-    <row r="1805" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1805" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1805" s="2" t="s">
         <v>123</v>
       </c>
@@ -74393,7 +74402,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1807" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1807" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1807" s="2" t="s">
         <v>102</v>
       </c>
@@ -75157,7 +75166,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="1827" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1827" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1827" t="s">
         <v>134</v>
       </c>
@@ -75655,7 +75664,7 @@
         <v>186.21814758489597</v>
       </c>
     </row>
-    <row r="1840" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1840" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1840" s="2" t="s">
         <v>1456</v>
       </c>
@@ -76343,7 +76352,12 @@
   <autoFilter ref="A1:M1857">
     <filterColumn colId="4">
       <filters>
-        <filter val="SNGLS"/>
+        <filter val="ETH"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="10">
+      <filters>
+        <filter val="Good +20%"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -76362,10 +76376,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M70"/>
+  <dimension ref="A1:M75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H70" sqref="H70"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -76376,8 +76391,9 @@
     <col min="4" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="160.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
@@ -78848,9 +78864,55 @@
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G70" t="s">
+        <v>1591</v>
+      </c>
       <c r="H70">
         <f>H69/G69</f>
         <v>1.3719999999999993E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G72" s="20" t="s">
+        <v>1592</v>
+      </c>
+      <c r="H72" s="19">
+        <f>H69*100</f>
+        <v>1439662.2379999992</v>
+      </c>
+      <c r="I72">
+        <f>H72/H75</f>
+        <v>4.9104970526945381E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G73" s="20" t="s">
+        <v>1593</v>
+      </c>
+      <c r="H73" s="19">
+        <f>H69*1000</f>
+        <v>14396622.379999992</v>
+      </c>
+      <c r="I73">
+        <f>H73/H74</f>
+        <v>0.34054682779305112</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G74" s="20" t="s">
+        <v>1594</v>
+      </c>
+      <c r="H74" s="19">
+        <v>42275015.372478403</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G75" s="20" t="s">
+        <v>1595</v>
+      </c>
+      <c r="H75" s="19">
+        <f>H74-H73+H72</f>
+        <v>29318055.23047841</v>
       </c>
     </row>
   </sheetData>

</xml_diff>